<commit_message>
Code for Mass Updates
</commit_message>
<xml_diff>
--- a/src/caseData.xlsx
+++ b/src/caseData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnarayan/Desktop/pgerDtyCaseMgmt/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B52A7323-8152-384F-8A78-ACD9DC753F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10C96919-BCED-F448-978D-ADE1D4606B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19580" yWindow="9900" windowWidth="28040" windowHeight="17440" xr2:uid="{05905B39-38D0-B348-B0B9-A0E73ECEAA34}"/>
   </bookViews>
@@ -35,12 +35,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>CaseId</t>
   </si>
   <si>
-    <t>Q25DE342BMDV7Y</t>
+    <t>Q39R6QGUYT990I</t>
+  </si>
+  <si>
+    <t>Q1Q1AJOH42BSXT</t>
+  </si>
+  <si>
+    <t>Q3RP3TDW2ZBAXV</t>
+  </si>
+  <si>
+    <t>Q228KVDG2DNUXC</t>
+  </si>
+  <si>
+    <t>Q2TJZ8SPTHNW6O</t>
+  </si>
+  <si>
+    <t>Q12CWO34LSXEUM</t>
+  </si>
+  <si>
+    <t>Q0F9BX3XYP7K9S</t>
+  </si>
+  <si>
+    <t>Q0UGGG4088I30I</t>
+  </si>
+  <si>
+    <t>Q07QM24SI5V8FO</t>
   </si>
 </sst>
 </file>
@@ -399,13 +423,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3E7408-985E-C040-B247-0AAAA362341E}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -417,6 +444,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>